<commit_message>
The changes in the PrivateCar.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr hidePivotFieldList="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar_SIT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE92AF23-47A7-4232-9AC5-3AE98898E8A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A19ABD8-D256-47CE-A75D-A13920A70555}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="221">
   <si>
     <t>Sno</t>
   </si>
@@ -634,36 +634,6 @@
     <t>29-03-2026</t>
   </si>
   <si>
-    <t>1000073464</t>
-  </si>
-  <si>
-    <t>Issued</t>
-  </si>
-  <si>
-    <t>Policy #00000402000070128</t>
-  </si>
-  <si>
-    <t>MYR 30199.00</t>
-  </si>
-  <si>
-    <t>MYR 319.44</t>
-  </si>
-  <si>
-    <t>MYR 1,211.87</t>
-  </si>
-  <si>
-    <t>MYR 302.97</t>
-  </si>
-  <si>
-    <t>MYR 908.90</t>
-  </si>
-  <si>
-    <t>MYR 72.71</t>
-  </si>
-  <si>
-    <t>MYR 991.61</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -685,36 +655,6 @@
     <t>19-03-2026</t>
   </si>
   <si>
-    <t>1000094383</t>
-  </si>
-  <si>
-    <t>Validated</t>
-  </si>
-  <si>
-    <t>Policy #-</t>
-  </si>
-  <si>
-    <t>MYR 23700.00</t>
-  </si>
-  <si>
-    <t>MYR 181.38</t>
-  </si>
-  <si>
-    <t>MYR 1,039.03</t>
-  </si>
-  <si>
-    <t>MYR 571.46</t>
-  </si>
-  <si>
-    <t>MYR 467.57</t>
-  </si>
-  <si>
-    <t>MYR 37.41</t>
-  </si>
-  <si>
-    <t>MYR 514.98</t>
-  </si>
-  <si>
     <t>Private Car Registered Vehicle</t>
   </si>
   <si>
@@ -737,12 +677,34 @@
   </si>
   <si>
     <t>740114025323</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>04-04-2025</t>
+  </si>
+  <si>
+    <t>03-04-2026</t>
+  </si>
+  <si>
+    <t>JGG1332</t>
+  </si>
+  <si>
+    <t>010128011227</t>
+  </si>
+  <si>
+    <t>11-05-2025</t>
+  </si>
+  <si>
+    <t>10-05-2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -11664,7 +11626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E49F7A5-BC9F-43C3-905D-E1A10F8B99B2}">
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
@@ -11672,17 +11634,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="29" width="9.140625" style="21"/>
-    <col min="30" max="30" width="15.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="3" max="29" style="21" width="9.140625"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="21" width="15.140625"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="32" max="16384" style="21" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="25" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -11744,7 +11706,7 @@
     </row>
     <row r="5" spans="1:31">
       <c r="AD5" s="22" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="AE5" s="23">
         <v>4</v>
@@ -11789,10 +11751,6 @@
       <c r="AE10" s="23">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:31">
-      <c r="AD11"/>
-      <c r="AE11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11808,47 +11766,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="36" width="24.140625" customWidth="1"/>
-    <col min="37" max="37" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="26" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.85546875" customWidth="1"/>
-    <col min="61" max="61" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="62.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.5703125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="20" width="13.140625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.42578125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5703125"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.85546875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="9.85546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.140625"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.28515625"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.85546875"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="4.42578125"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="24.140625"/>
+    <col min="27" max="36" customWidth="true" width="24.140625"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="19.5703125"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" width="26.0"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="29.140625"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="28.28515625"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
+    <col min="60" max="60" customWidth="true" width="10.85546875"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="16.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="9" customFormat="1" ht="31.5">
@@ -12033,7 +11991,7 @@
         <v>191</v>
       </c>
       <c r="BI1" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:61" ht="72">
@@ -12047,25 +12005,25 @@
         <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>230</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -12073,48 +12031,20 @@
       <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
       <c r="AA2" s="3" t="s">
         <v>114</v>
       </c>
@@ -12125,7 +12055,7 @@
         <v>116</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>116</v>
@@ -12194,7 +12124,7 @@
         <v>194</v>
       </c>
       <c r="BI2" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:61" ht="72">
@@ -12208,7 +12138,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -12220,13 +12150,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -12234,48 +12164,20 @@
       <c r="L3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>225</v>
-      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
       <c r="AA3" s="3" t="s">
         <v>26</v>
       </c>
@@ -12286,7 +12188,7 @@
         <v>66</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>66</v>
@@ -12355,7 +12257,7 @@
         <v>194</v>
       </c>
       <c r="BI3" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:61" ht="72">
@@ -12369,7 +12271,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -12381,13 +12283,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>233</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -12460,7 +12362,7 @@
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
       <c r="AY4" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ4" s="3" t="s">
         <v>40</v>
@@ -12488,7 +12390,7 @@
         <v>194</v>
       </c>
       <c r="BI4" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:61" ht="72">
@@ -12502,7 +12404,7 @@
         <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -12520,7 +12422,7 @@
         <v>196</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -12593,7 +12495,7 @@
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
       <c r="AY5" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ5" s="3" t="s">
         <v>40</v>
@@ -12621,7 +12523,7 @@
         <v>194</v>
       </c>
       <c r="BI5" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:61" ht="72">
@@ -12635,13 +12537,13 @@
         <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>230</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
@@ -12649,7 +12551,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -12722,7 +12624,7 @@
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
       <c r="AY6" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ6" s="3" t="s">
         <v>40</v>
@@ -12750,7 +12652,7 @@
         <v>194</v>
       </c>
       <c r="BI6" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:61" ht="72">
@@ -12764,13 +12666,13 @@
         <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -12782,7 +12684,7 @@
         <v>198</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -12855,7 +12757,7 @@
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
       <c r="AY7" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ7" s="3" t="s">
         <v>40</v>
@@ -12883,7 +12785,7 @@
         <v>194</v>
       </c>
       <c r="BI7" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:61" ht="72">
@@ -12897,13 +12799,13 @@
         <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>230</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -12911,7 +12813,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
       <c r="J8" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -12984,7 +12886,7 @@
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
       <c r="AY8" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ8" s="3" t="s">
         <v>40</v>
@@ -13012,7 +12914,7 @@
         <v>194</v>
       </c>
       <c r="BI8" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:61" ht="72">
@@ -13026,7 +12928,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>92</v>
@@ -13040,7 +12942,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
       <c r="J9" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -13113,7 +13015,7 @@
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
       <c r="AY9" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ9" s="3" t="s">
         <v>40</v>
@@ -13141,7 +13043,7 @@
         <v>194</v>
       </c>
       <c r="BI9" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:61" ht="72">
@@ -13155,7 +13057,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -13169,7 +13071,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
       <c r="J10" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -13242,7 +13144,7 @@
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
       <c r="AY10" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ10" s="3" t="s">
         <v>40</v>
@@ -13270,7 +13172,7 @@
         <v>194</v>
       </c>
       <c r="BI10" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:61" ht="72">
@@ -13284,7 +13186,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>56</v>
@@ -13298,7 +13200,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
       <c r="J11" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -13371,7 +13273,7 @@
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
       <c r="AY11" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ11" s="3" t="s">
         <v>40</v>
@@ -13399,7 +13301,7 @@
         <v>194</v>
       </c>
       <c r="BI11" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:61" ht="72">
@@ -13413,7 +13315,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>89</v>
@@ -13427,7 +13329,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
       <c r="J12" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -13500,7 +13402,7 @@
       <c r="AW12" s="3"/>
       <c r="AX12" s="3"/>
       <c r="AY12" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ12" s="3" t="s">
         <v>40</v>
@@ -13528,7 +13430,7 @@
         <v>194</v>
       </c>
       <c r="BI12" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:61" ht="72">
@@ -13542,13 +13444,13 @@
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>230</v>
+        <v>176</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -13556,7 +13458,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="3"/>
       <c r="J13" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>
@@ -13629,7 +13531,7 @@
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="AZ13" s="3" t="s">
         <v>40</v>
@@ -13657,7 +13559,7 @@
         <v>194</v>
       </c>
       <c r="BI13" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -13676,14 +13578,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="3" max="16384" style="21" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="25" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -13802,11 +13704,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="31.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" style="20"/>
-    <col min="51" max="51" width="27" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="9.85546875"/>
+    <col min="3" max="3" customWidth="true" width="35.85546875"/>
+    <col min="11" max="11" customWidth="true" width="18.5703125"/>
+    <col min="13" max="13" style="20" width="24.7109375"/>
+    <col min="51" max="51" customWidth="true" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="31.5" customHeight="1">
@@ -15911,17 +15813,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="30" width="9.140625" style="21"/>
-    <col min="31" max="31" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="3" max="30" style="21" width="9.140625"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="33" max="16384" style="21" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" s="25" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -16040,22 +15942,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="3" max="3" customWidth="true" width="22.0"/>
+    <col min="4" max="4" customWidth="true" width="13.0"/>
+    <col min="5" max="5" customWidth="true" width="14.0"/>
+    <col min="6" max="6" customWidth="true" width="15.7109375"/>
+    <col min="7" max="7" customWidth="true" width="14.7109375"/>
+    <col min="8" max="8" customWidth="true" width="15.0"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125"/>
+    <col min="10" max="10" customWidth="true" width="14.0"/>
+    <col min="11" max="11" customWidth="true" width="13.5703125"/>
+    <col min="12" max="12" customWidth="true" width="13.0"/>
+    <col min="13" max="13" customWidth="true" width="17.5703125"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="16.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:60" ht="31.5">
@@ -16251,7 +16153,7 @@
         <v>175</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -16265,7 +16167,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -16377,7 +16279,7 @@
         <v>175</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -16393,7 +16295,7 @@
         <v>178</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -16505,7 +16407,7 @@
         <v>175</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -16519,7 +16421,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
       <c r="J4" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -16631,7 +16533,7 @@
         <v>175</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -16647,7 +16549,7 @@
         <v>178</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -16759,7 +16661,7 @@
         <v>175</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>89</v>
@@ -16773,7 +16675,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -16885,7 +16787,7 @@
         <v>175</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>92</v>
@@ -16897,7 +16799,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -17009,7 +16911,7 @@
         <v>175</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
@@ -17023,7 +16925,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
       <c r="J8" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -17135,7 +17037,7 @@
         <v>175</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>92</v>
@@ -17147,7 +17049,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
       <c r="J9" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -17259,7 +17161,7 @@
         <v>175</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -17273,7 +17175,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
       <c r="J10" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -17385,7 +17287,7 @@
         <v>175</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>56</v>
@@ -17397,7 +17299,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
       <c r="J11" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -17509,7 +17411,7 @@
         <v>175</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>89</v>
@@ -17523,7 +17425,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
       <c r="J12" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -17635,7 +17537,7 @@
         <v>175</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>92</v>
@@ -17647,7 +17549,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="3"/>
       <c r="J13" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
The pdf file is downloaded to directory in local project [QuoteLetter]
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="223">
   <si>
     <t>Sno</t>
   </si>
@@ -698,6 +698,12 @@
   </si>
   <si>
     <t>10-05-2026</t>
+  </si>
+  <si>
+    <t>30-04-2025</t>
+  </si>
+  <si>
+    <t>29-04-2026</t>
   </si>
 </sst>
 </file>
@@ -16164,8 +16170,12 @@
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>222</v>
+      </c>
       <c r="J2" s="4" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
The code for policy schedule downloading in added successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A19ABD8-D256-47CE-A75D-A13920A70555}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6796D815-4A44-4759-9705-ABABC4C02C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DashboardRV" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="268">
   <si>
     <t>Sno</t>
   </si>
@@ -640,21 +640,12 @@
     <t>940630123455</t>
   </si>
   <si>
-    <t>VGA6536</t>
-  </si>
-  <si>
     <t>21-04-2025</t>
   </si>
   <si>
     <t>20-04-2026</t>
   </si>
   <si>
-    <t>20-03-2025</t>
-  </si>
-  <si>
-    <t>19-03-2026</t>
-  </si>
-  <si>
     <t>Private Car Registered Vehicle</t>
   </si>
   <si>
@@ -673,37 +664,181 @@
     <t>PLAN A</t>
   </si>
   <si>
-    <t>PKF3988</t>
-  </si>
-  <si>
-    <t>740114025323</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>04-04-2025</t>
-  </si>
-  <si>
-    <t>03-04-2026</t>
-  </si>
-  <si>
-    <t>JGG1332</t>
-  </si>
-  <si>
-    <t>010128011227</t>
-  </si>
-  <si>
     <t>11-05-2025</t>
   </si>
   <si>
     <t>10-05-2026</t>
   </si>
   <si>
-    <t>30-04-2025</t>
-  </si>
-  <si>
-    <t>29-04-2026</t>
+    <t>03-05-2025</t>
+  </si>
+  <si>
+    <t>02-05-2026</t>
+  </si>
+  <si>
+    <t>WYQ9503</t>
+  </si>
+  <si>
+    <t>971119016061</t>
+  </si>
+  <si>
+    <t>04-05-2025</t>
+  </si>
+  <si>
+    <t>03-05-2026</t>
+  </si>
+  <si>
+    <t>1000032212</t>
+  </si>
+  <si>
+    <t>Issued</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047279</t>
+  </si>
+  <si>
+    <t>MYR 43733.00</t>
+  </si>
+  <si>
+    <t>MYR 381.36</t>
+  </si>
+  <si>
+    <t>MYR 1,637.03</t>
+  </si>
+  <si>
+    <t>- MYR 0.00</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>MYR 130.96</t>
+  </si>
+  <si>
+    <t>MYR 1,777.99</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>1000032216</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047281</t>
+  </si>
+  <si>
+    <t>MYR 44166.00</t>
+  </si>
+  <si>
+    <t>MYR 385.45</t>
+  </si>
+  <si>
+    <t>MYR 1,666.93</t>
+  </si>
+  <si>
+    <t>MYR 133.35</t>
+  </si>
+  <si>
+    <t>MYR 1,810.28</t>
+  </si>
+  <si>
+    <t>1000032217</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047282</t>
+  </si>
+  <si>
+    <t>MYR 44599.00</t>
+  </si>
+  <si>
+    <t>1000032218</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047283</t>
+  </si>
+  <si>
+    <t>MYR 45032.00</t>
+  </si>
+  <si>
+    <t>MYR 390.29</t>
+  </si>
+  <si>
+    <t>MYR 1,696.83</t>
+  </si>
+  <si>
+    <t>MYR 135.75</t>
+  </si>
+  <si>
+    <t>MYR 1,842.58</t>
+  </si>
+  <si>
+    <t>1000032223</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047285</t>
+  </si>
+  <si>
+    <t>MYR 45465.00</t>
+  </si>
+  <si>
+    <t>1000032224</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047286</t>
+  </si>
+  <si>
+    <t>MYR 45898.00</t>
+  </si>
+  <si>
+    <t>06-05-2025</t>
+  </si>
+  <si>
+    <t>05-05-2026</t>
+  </si>
+  <si>
+    <t>1000032265</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047312</t>
+  </si>
+  <si>
+    <t>MYR 29189.00</t>
+  </si>
+  <si>
+    <t>MYR 424.93</t>
+  </si>
+  <si>
+    <t>MYR 1,401.19</t>
+  </si>
+  <si>
+    <t>MYR 112.10</t>
+  </si>
+  <si>
+    <t>MYR 1,523.29</t>
+  </si>
+  <si>
+    <t>1000032269</t>
+  </si>
+  <si>
+    <t>Policy #00000402000047315</t>
+  </si>
+  <si>
+    <t>MYR 28900.00</t>
+  </si>
+  <si>
+    <t>MYR 428.59</t>
+  </si>
+  <si>
+    <t>MYR 1,366.80</t>
+  </si>
+  <si>
+    <t>MYR 109.34</t>
+  </si>
+  <si>
+    <t>MYR 1,486.14</t>
   </si>
 </sst>
 </file>
@@ -10755,6 +10890,148 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E65630C9-EB18-432C-A1B4-98C52238F2EB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="AF14:AG16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="68">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="61"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="65" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="17">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea field="61" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="61" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{591533EA-EEAC-4542-9EEA-CD8FE30E3B88}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AF9:AG12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="68">
@@ -10854,26 +11131,26 @@
     <dataField name="Sum of Value" fld="65" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="17">
+    <format dxfId="23">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="21">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="17" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -10924,280 +11201,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E65630C9-EB18-432C-A1B4-98C52238F2EB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="AF14:AG16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="68">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="61"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="65" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="23">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="21">
-      <pivotArea field="61" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="61" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4835F9D5-316A-469B-AC80-1739299B9E0F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="AE14:AF16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="57">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="49"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="5">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="3">
-      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="49" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{237DE21D-C108-407B-9CCD-EB11944F6790}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AE9:AF12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="57">
@@ -11287,26 +11291,26 @@
     <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="11">
+    <format dxfId="5">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="3">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -11352,6 +11356,137 @@
           </reference>
           <reference field="5" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4835F9D5-316A-469B-AC80-1739299B9E0F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="AE14:AF16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="57">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="49"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="11">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="49" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -11650,7 +11785,7 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="25" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -11712,7 +11847,7 @@
     </row>
     <row r="5" spans="1:31">
       <c r="AD5" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AE5" s="23">
         <v>4</v>
@@ -11772,8 +11907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11997,7 +12132,7 @@
         <v>191</v>
       </c>
       <c r="BI1" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:61" ht="72">
@@ -12011,7 +12146,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -12023,13 +12158,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>219</v>
+        <v>252</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>220</v>
+        <v>253</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -12037,20 +12172,48 @@
       <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="AA2" s="3" t="s">
         <v>114</v>
       </c>
@@ -12090,17 +12253,39 @@
       <c r="AM2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
+      <c r="AN2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY2" s="3" t="s">
         <v>29</v>
       </c>
@@ -12130,7 +12315,7 @@
         <v>194</v>
       </c>
       <c r="BI2" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:61" ht="72">
@@ -12144,25 +12329,25 @@
         <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>176</v>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -12263,7 +12448,7 @@
         <v>194</v>
       </c>
       <c r="BI3" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:61" ht="72">
@@ -12277,7 +12462,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -12289,13 +12474,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="J4" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -12368,7 +12553,7 @@
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
       <c r="AY4" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ4" s="3" t="s">
         <v>40</v>
@@ -12396,7 +12581,7 @@
         <v>194</v>
       </c>
       <c r="BI4" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:61" ht="72">
@@ -12410,13 +12595,13 @@
         <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>176</v>
+      <c r="F5" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -12428,7 +12613,7 @@
         <v>196</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -12501,7 +12686,7 @@
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
       <c r="AY5" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ5" s="3" t="s">
         <v>40</v>
@@ -12529,7 +12714,7 @@
         <v>194</v>
       </c>
       <c r="BI5" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:61" ht="72">
@@ -12543,7 +12728,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>89</v>
@@ -12557,7 +12742,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -12630,7 +12815,7 @@
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
       <c r="AY6" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ6" s="3" t="s">
         <v>40</v>
@@ -12658,7 +12843,7 @@
         <v>194</v>
       </c>
       <c r="BI6" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:61" ht="72">
@@ -12672,13 +12857,13 @@
         <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>176</v>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -12690,7 +12875,7 @@
         <v>198</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -12763,7 +12948,7 @@
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
       <c r="AY7" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ7" s="3" t="s">
         <v>40</v>
@@ -12791,7 +12976,7 @@
         <v>194</v>
       </c>
       <c r="BI7" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:61" ht="72">
@@ -12805,7 +12990,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
@@ -12819,7 +13004,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
       <c r="J8" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -12892,7 +13077,7 @@
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
       <c r="AY8" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ8" s="3" t="s">
         <v>40</v>
@@ -12920,7 +13105,7 @@
         <v>194</v>
       </c>
       <c r="BI8" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:61" ht="72">
@@ -12934,13 +13119,13 @@
         <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>176</v>
+      <c r="F9" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
@@ -12948,7 +13133,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
       <c r="J9" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -13021,7 +13206,7 @@
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
       <c r="AY9" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ9" s="3" t="s">
         <v>40</v>
@@ -13049,7 +13234,7 @@
         <v>194</v>
       </c>
       <c r="BI9" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:61" ht="72">
@@ -13063,7 +13248,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -13077,7 +13262,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
       <c r="J10" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -13150,7 +13335,7 @@
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
       <c r="AY10" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ10" s="3" t="s">
         <v>40</v>
@@ -13178,7 +13363,7 @@
         <v>194</v>
       </c>
       <c r="BI10" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:61" ht="72">
@@ -13192,13 +13377,13 @@
         <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>176</v>
+      <c r="F11" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
@@ -13206,7 +13391,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
       <c r="J11" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -13279,7 +13464,7 @@
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
       <c r="AY11" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ11" s="3" t="s">
         <v>40</v>
@@ -13307,7 +13492,7 @@
         <v>194</v>
       </c>
       <c r="BI11" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:61" ht="72">
@@ -13321,7 +13506,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>89</v>
@@ -13335,7 +13520,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
       <c r="J12" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -13408,7 +13593,7 @@
       <c r="AW12" s="3"/>
       <c r="AX12" s="3"/>
       <c r="AY12" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ12" s="3" t="s">
         <v>40</v>
@@ -13436,7 +13621,7 @@
         <v>194</v>
       </c>
       <c r="BI12" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:61" ht="72">
@@ -13450,13 +13635,13 @@
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>176</v>
+      <c r="F13" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -13464,7 +13649,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="3"/>
       <c r="J13" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>
@@ -13537,7 +13722,7 @@
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AZ13" s="3" t="s">
         <v>40</v>
@@ -13565,7 +13750,7 @@
         <v>194</v>
       </c>
       <c r="BI13" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -13591,7 +13776,7 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="25" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -15829,7 +16014,7 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" s="25" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -15942,8 +16127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D5A56-986F-42E7-8D16-7CE6B8C79095}">
   <dimension ref="A1:BH13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16159,7 +16344,7 @@
         <v>175</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -16171,10 +16356,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>200</v>
@@ -16185,20 +16370,48 @@
       <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>260</v>
+      </c>
       <c r="AA2" s="3" t="s">
         <v>114</v>
       </c>
@@ -16238,17 +16451,39 @@
       <c r="AM2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
+      <c r="AN2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY2" s="3" t="s">
         <v>29</v>
       </c>
@@ -16289,7 +16524,7 @@
         <v>175</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -16417,7 +16652,7 @@
         <v>175</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -16428,8 +16663,12 @@
       <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="J4" s="4" t="s">
         <v>200</v>
       </c>
@@ -16439,20 +16678,48 @@
       <c r="L4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
+      <c r="M4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="AA4" s="3" t="s">
         <v>58</v>
       </c>
@@ -16492,17 +16759,39 @@
       <c r="AM4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN4" s="3"/>
-      <c r="AO4" s="3"/>
-      <c r="AP4" s="3"/>
-      <c r="AQ4" s="3"/>
-      <c r="AR4" s="3"/>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AV4" s="3"/>
-      <c r="AW4" s="3"/>
-      <c r="AX4" s="3"/>
+      <c r="AN4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW4" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX4" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY4" s="3" t="s">
         <v>29</v>
       </c>
@@ -16543,7 +16832,7 @@
         <v>175</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -16671,7 +16960,7 @@
         <v>175</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>89</v>
@@ -16682,8 +16971,12 @@
       <c r="G6" s="2">
         <v>3</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>200</v>
       </c>
@@ -16693,20 +16986,48 @@
       <c r="L6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="AA6" s="3" t="s">
         <v>71</v>
       </c>
@@ -16746,17 +17067,39 @@
       <c r="AM6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="3"/>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="3"/>
-      <c r="AU6" s="3"/>
-      <c r="AV6" s="3"/>
-      <c r="AW6" s="3"/>
-      <c r="AX6" s="3"/>
+      <c r="AN6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX6" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY6" s="3" t="s">
         <v>29</v>
       </c>
@@ -16797,7 +17140,7 @@
         <v>175</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>92</v>
@@ -16921,7 +17264,7 @@
         <v>175</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
@@ -16932,8 +17275,12 @@
       <c r="G8" s="2">
         <v>4</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="J8" s="4" t="s">
         <v>200</v>
       </c>
@@ -16943,20 +17290,48 @@
       <c r="L8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
+      <c r="M8" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="AA8" s="3" t="s">
         <v>82</v>
       </c>
@@ -16996,17 +17371,39 @@
       <c r="AM8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AP8" s="3"/>
-      <c r="AQ8" s="3"/>
-      <c r="AR8" s="3"/>
-      <c r="AS8" s="3"/>
-      <c r="AT8" s="3"/>
-      <c r="AU8" s="3"/>
-      <c r="AV8" s="3"/>
-      <c r="AW8" s="3"/>
-      <c r="AX8" s="3"/>
+      <c r="AN8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS8" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU8" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW8" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX8" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY8" s="3" t="s">
         <v>29</v>
       </c>
@@ -17047,7 +17444,7 @@
         <v>175</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>92</v>
@@ -17171,7 +17568,7 @@
         <v>175</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -17182,8 +17579,12 @@
       <c r="G10" s="2">
         <v>5</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>200</v>
       </c>
@@ -17193,20 +17594,48 @@
       <c r="L10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="AA10" s="3" t="s">
         <v>120</v>
       </c>
@@ -17246,17 +17675,39 @@
       <c r="AM10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="3"/>
-      <c r="AQ10" s="3"/>
-      <c r="AR10" s="3"/>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="3"/>
-      <c r="AU10" s="3"/>
-      <c r="AV10" s="3"/>
-      <c r="AW10" s="3"/>
-      <c r="AX10" s="3"/>
+      <c r="AN10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX10" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY10" s="3" t="s">
         <v>29</v>
       </c>
@@ -17297,7 +17748,7 @@
         <v>175</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>56</v>
@@ -17421,7 +17872,7 @@
         <v>175</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>89</v>
@@ -17432,8 +17883,12 @@
       <c r="G12" s="2">
         <v>6</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="J12" s="4" t="s">
         <v>200</v>
       </c>
@@ -17443,20 +17898,48 @@
       <c r="L12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="AA12" s="3" t="s">
         <v>127</v>
       </c>
@@ -17496,17 +17979,39 @@
       <c r="AM12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
-      <c r="AP12" s="3"/>
-      <c r="AQ12" s="3"/>
-      <c r="AR12" s="3"/>
-      <c r="AS12" s="3"/>
-      <c r="AT12" s="3"/>
-      <c r="AU12" s="3"/>
-      <c r="AV12" s="3"/>
-      <c r="AW12" s="3"/>
-      <c r="AX12" s="3"/>
+      <c r="AN12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS12" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU12" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW12" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX12" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="AY12" s="3" t="s">
         <v>29</v>
       </c>
@@ -17547,7 +18052,7 @@
         <v>175</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
The motor tile changes after CV deployment
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BDCF6C-25A2-4CF3-9F28-AE4172AE130C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685DB1FF-F5D4-489A-A0FC-564B5D0F2E10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="288">
   <si>
     <t>Sno</t>
   </si>
@@ -658,9 +658,6 @@
     <t>146</t>
   </si>
   <si>
-    <t>MYR 268.30</t>
-  </si>
-  <si>
     <t>MYR 470.93</t>
   </si>
   <si>
@@ -694,108 +691,24 @@
     <t>MYR 643.64</t>
   </si>
   <si>
-    <t>1000034209</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048779</t>
-  </si>
-  <si>
-    <t>990902016892</t>
-  </si>
-  <si>
     <t>MYR 366.84</t>
   </si>
   <si>
-    <t>AJH151</t>
-  </si>
-  <si>
-    <t>011001060309</t>
-  </si>
-  <si>
-    <t>BNE7319</t>
-  </si>
-  <si>
-    <t>760728145379</t>
-  </si>
-  <si>
-    <t>MYR 261.17</t>
-  </si>
-  <si>
-    <t>1000034603</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048930</t>
-  </si>
-  <si>
-    <t>1000034604</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048931</t>
-  </si>
-  <si>
     <t>MYR 323.63</t>
   </si>
   <si>
-    <t>1000034605</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048932</t>
-  </si>
-  <si>
-    <t>1000034606</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048933</t>
-  </si>
-  <si>
-    <t>1000034607</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048934</t>
-  </si>
-  <si>
-    <t>1000034608</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048935</t>
-  </si>
-  <si>
-    <t>1000034610</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048936</t>
-  </si>
-  <si>
-    <t>1000034611</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048937</t>
-  </si>
-  <si>
     <t>1000034612</t>
   </si>
   <si>
     <t>Policy #00000402000048938</t>
   </si>
   <si>
-    <t>1000034613</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048939</t>
-  </si>
-  <si>
     <t>25-05-2025</t>
   </si>
   <si>
     <t>24-05-2026</t>
   </si>
   <si>
-    <t>1000034615</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048941</t>
-  </si>
-  <si>
     <t>MYR 24500.00</t>
   </si>
   <si>
@@ -811,12 +724,6 @@
     <t>MYR 1,337.60</t>
   </si>
   <si>
-    <t>1000034616</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048942</t>
-  </si>
-  <si>
     <t>MYR 30800.00</t>
   </si>
   <si>
@@ -832,148 +739,103 @@
     <t>MYR 1,358.20</t>
   </si>
   <si>
-    <t>1000034632</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048951</t>
-  </si>
-  <si>
-    <t>1000034635</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048954</t>
-  </si>
-  <si>
-    <t>1000034639</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048957</t>
-  </si>
-  <si>
-    <t>1000034641</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048959</t>
-  </si>
-  <si>
-    <t>1000034647</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048962</t>
-  </si>
-  <si>
-    <t>1000034649</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048965</t>
-  </si>
-  <si>
-    <t>1000034653</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048967</t>
-  </si>
-  <si>
-    <t>1000034658</t>
-  </si>
-  <si>
-    <t>Policy #00000402000048971</t>
-  </si>
-  <si>
-    <t>1000034778</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049094</t>
-  </si>
-  <si>
-    <t>1000034781</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049096</t>
-  </si>
-  <si>
-    <t>1000034784</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049098</t>
-  </si>
-  <si>
-    <t>1000034785</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049100</t>
-  </si>
-  <si>
-    <t>1000034786</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049101</t>
-  </si>
-  <si>
-    <t>1000034787</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049102</t>
-  </si>
-  <si>
-    <t>1000034788</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049103</t>
-  </si>
-  <si>
-    <t>1000034791</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049105</t>
-  </si>
-  <si>
-    <t>1000034792</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049106</t>
-  </si>
-  <si>
-    <t>1000034794</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049108</t>
-  </si>
-  <si>
-    <t>1000034795</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049109</t>
-  </si>
-  <si>
-    <t>27-05-2025</t>
-  </si>
-  <si>
-    <t>26-05-2026</t>
-  </si>
-  <si>
-    <t>1000034837</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049154</t>
-  </si>
-  <si>
     <t>951126115254</t>
   </si>
   <si>
-    <t>28-05-2025</t>
-  </si>
-  <si>
-    <t>27-05-2026</t>
-  </si>
-  <si>
-    <t>1000034963</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049288</t>
-  </si>
-  <si>
-    <t>1000034967</t>
+    <t>MYR 267.30</t>
+  </si>
+  <si>
+    <t>29-05-2025</t>
+  </si>
+  <si>
+    <t>28-05-2026</t>
+  </si>
+  <si>
+    <t>MYR 364.97</t>
+  </si>
+  <si>
+    <t>1000035101</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049390</t>
+  </si>
+  <si>
+    <t>1000035103</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049391</t>
+  </si>
+  <si>
+    <t>MYR 318.65</t>
+  </si>
+  <si>
+    <t>1000035105</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049392</t>
+  </si>
+  <si>
+    <t>MYR 259.79</t>
+  </si>
+  <si>
+    <t>1000035106</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049394</t>
+  </si>
+  <si>
+    <t>1000035108</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049396</t>
+  </si>
+  <si>
+    <t>1000035110</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049397</t>
+  </si>
+  <si>
+    <t>1000035113</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049398</t>
+  </si>
+  <si>
+    <t>1000035117</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049401</t>
+  </si>
+  <si>
+    <t>1000035121</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049404</t>
+  </si>
+  <si>
+    <t>1000035123</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049407</t>
+  </si>
+  <si>
+    <t>MYR 10201.00</t>
+  </si>
+  <si>
+    <t>MYR 165.13</t>
+  </si>
+  <si>
+    <t>MYR 532.89</t>
+  </si>
+  <si>
+    <t>MYR 42.63</t>
+  </si>
+  <si>
+    <t>MYR 585.52</t>
+  </si>
+  <si>
+    <t>1000035211</t>
   </si>
   <si>
     <t>Validated</t>
@@ -982,7 +844,61 @@
     <t>Policy #-</t>
   </si>
   <si>
-    <t>MYR 267.30</t>
+    <t>QAR8405</t>
+  </si>
+  <si>
+    <t>940309135537</t>
+  </si>
+  <si>
+    <t>1000035321</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049593</t>
+  </si>
+  <si>
+    <t>MYR 369.66</t>
+  </si>
+  <si>
+    <t>03-06-2025</t>
+  </si>
+  <si>
+    <t>02-06-2026</t>
+  </si>
+  <si>
+    <t>1000035464</t>
+  </si>
+  <si>
+    <t>Policy #00000402000049666</t>
+  </si>
+  <si>
+    <t>MYR 8300.00</t>
+  </si>
+  <si>
+    <t>MYR 288.86</t>
+  </si>
+  <si>
+    <t>MYR 637.18</t>
+  </si>
+  <si>
+    <t>MYR 50.97</t>
+  </si>
+  <si>
+    <t>MYR 698.15</t>
+  </si>
+  <si>
+    <t>020215011574</t>
+  </si>
+  <si>
+    <t>630319115042</t>
+  </si>
+  <si>
+    <t>04-06-2025</t>
+  </si>
+  <si>
+    <t>03-06-2026</t>
+  </si>
+  <si>
+    <t>960418016893</t>
   </si>
 </sst>
 </file>
@@ -10714,138 +10630,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AED3F0BB-4395-4CA7-89EB-11170616EB3B}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="AD8:AE10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="57">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="49"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="29">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="28">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="27">
-      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="26">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="49" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F42B4656-5BD3-4AA6-9202-8933937E4AB3}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AD3:AE7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="57">
@@ -10939,26 +10723,26 @@
     <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="35">
+    <format dxfId="29">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="28">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="27">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -11016,6 +10800,138 @@
           </reference>
           <reference field="5" count="1" selected="0">
             <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AED3F0BB-4395-4CA7-89EB-11170616EB3B}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="AD8:AE10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="57">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item m="1" x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="49"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="35">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="34">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="33">
+      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="49" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -12051,8 +11967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12293,7 +12209,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -12305,13 +12221,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>224</v>
+        <v>287</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -12320,46 +12236,46 @@
         <v>3</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>190</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>114</v>
@@ -12431,7 +12347,7 @@
         <v>192</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>29</v>
@@ -12479,7 +12395,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -12491,13 +12407,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>304</v>
+        <v>275</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>224</v>
+        <v>287</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -12505,47 +12421,41 @@
       <c r="L3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="AA3" s="3" t="s">
         <v>26</v>
@@ -12665,7 +12575,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -12677,13 +12587,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -12691,47 +12601,41 @@
       <c r="L4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>259</v>
-      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>58</v>
@@ -12851,7 +12755,7 @@
         <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -12863,13 +12767,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -12877,47 +12781,41 @@
       <c r="L5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="U5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>26</v>
@@ -13037,7 +12935,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>89</v>
@@ -13049,13 +12947,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -13063,47 +12961,41 @@
       <c r="L6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="U6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="W6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="Y6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="AA6" s="3" t="s">
         <v>71</v>
@@ -13223,7 +13115,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>92</v>
@@ -13235,13 +13127,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -13249,47 +13141,41 @@
       <c r="L7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>268</v>
-      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
       <c r="P7" s="3" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="W7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="Y7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="AA7" s="3" t="s">
         <v>26</v>
@@ -13409,7 +13295,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
@@ -13421,13 +13307,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -13435,47 +13321,41 @@
       <c r="L8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="W8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="Y8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="AA8" s="3" t="s">
         <v>82</v>
@@ -13595,7 +13475,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>92</v>
@@ -13607,13 +13487,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -13621,47 +13501,41 @@
       <c r="L9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>272</v>
-      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="U9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="W9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="Y9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="AA9" s="3" t="s">
         <v>26</v>
@@ -13781,7 +13655,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -13793,13 +13667,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -13807,47 +13681,41 @@
       <c r="L10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>274</v>
-      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="U10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="W10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="Y10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="AA10" s="3" t="s">
         <v>120</v>
@@ -13967,7 +13835,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>56</v>
@@ -13979,13 +13847,13 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -13993,47 +13861,41 @@
       <c r="L11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>276</v>
-      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="W11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="Y11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="AA11" s="3" t="s">
         <v>26</v>
@@ -14153,7 +14015,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>89</v>
@@ -14165,13 +14027,13 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -14179,47 +14041,41 @@
       <c r="L12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>278</v>
-      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="U12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="W12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="Y12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>127</v>
@@ -14339,7 +14195,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>92</v>
@@ -14351,13 +14207,13 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>
@@ -14365,47 +14221,41 @@
       <c r="L13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>280</v>
-      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
       <c r="P13" s="3" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="U13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="W13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="Y13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="AA13" s="3" t="s">
         <v>26</v>
@@ -14939,7 +14789,7 @@
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
       <c r="V2" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>37</v>
@@ -14948,46 +14798,46 @@
         <v>153</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>312</v>
+        <v>239</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>314</v>
+        <v>240</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>315</v>
+        <v>235</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM2" s="3" t="s">
         <v>148</v>
@@ -15146,7 +14996,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>37</v>
@@ -15155,46 +15005,46 @@
         <v>153</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="AB3" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM3" s="3" t="s">
         <v>148</v>
@@ -15236,7 +15086,7 @@
         <v>34</v>
       </c>
       <c r="AZ3" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA3" s="3" t="s">
         <v>183</v>
@@ -15355,7 +15205,7 @@
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W4" s="5" t="s">
         <v>37</v>
@@ -15364,46 +15214,46 @@
         <v>153</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM4" s="3" t="s">
         <v>148</v>
@@ -15562,7 +15412,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W5" s="5" t="s">
         <v>37</v>
@@ -15571,46 +15421,46 @@
         <v>153</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="AB5" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE5" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM5" s="3" t="s">
         <v>148</v>
@@ -15652,7 +15502,7 @@
         <v>34</v>
       </c>
       <c r="AZ5" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA5" s="3" t="s">
         <v>183</v>
@@ -15771,7 +15621,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W6" s="5" t="s">
         <v>37</v>
@@ -15780,46 +15630,46 @@
         <v>153</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>237</v>
+        <v>266</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>211</v>
+        <v>267</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="AB6" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC6" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="AE6" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM6" s="3" t="s">
         <v>148</v>
@@ -15861,7 +15711,7 @@
         <v>34</v>
       </c>
       <c r="AZ6" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA6" s="3" t="s">
         <v>183</v>
@@ -15978,7 +15828,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W7" s="5" t="s">
         <v>37</v>
@@ -15987,46 +15837,46 @@
         <v>153</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="AB7" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="AD7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE7" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL7" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM7" s="3" t="s">
         <v>148</v>
@@ -16068,7 +15918,7 @@
         <v>34</v>
       </c>
       <c r="AZ7" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA7" s="3" t="s">
         <v>183</v>
@@ -16187,7 +16037,7 @@
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="V8" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W8" s="5" t="s">
         <v>37</v>
@@ -16195,20 +16045,48 @@
       <c r="X8" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
+      <c r="Y8" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AK8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="AM8" s="3" t="s">
         <v>148</v>
       </c>
@@ -16242,21 +16120,45 @@
       <c r="AW8" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="AX8" s="3"/>
+      <c r="AX8" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="AY8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AZ8" s="3"/>
-      <c r="BA8" s="3"/>
-      <c r="BB8" s="3"/>
-      <c r="BC8" s="3"/>
-      <c r="BD8" s="3"/>
-      <c r="BE8" s="3"/>
-      <c r="BF8" s="3"/>
-      <c r="BG8" s="3"/>
-      <c r="BH8" s="3"/>
-      <c r="BI8" s="3"/>
-      <c r="BJ8" s="3"/>
+      <c r="AZ8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BA8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BB8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BE8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BF8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BG8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BH8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BI8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BJ8" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="BK8" s="3" t="s">
         <v>29</v>
       </c>
@@ -16342,7 +16244,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W9" s="5" t="s">
         <v>37</v>
@@ -16351,46 +16253,46 @@
         <v>153</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="AB9" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="AD9" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE9" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH9" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL9" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM9" s="3" t="s">
         <v>148</v>
@@ -16432,7 +16334,7 @@
         <v>34</v>
       </c>
       <c r="AZ9" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA9" s="3" t="s">
         <v>183</v>
@@ -16551,7 +16453,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W10" s="5" t="s">
         <v>37</v>
@@ -16560,46 +16462,46 @@
         <v>153</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="AB10" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC10" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD10" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="AD10" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="AE10" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF10" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH10" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL10" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM10" s="3" t="s">
         <v>148</v>
@@ -16641,7 +16543,7 @@
         <v>34</v>
       </c>
       <c r="AZ10" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA10" s="3" t="s">
         <v>183</v>
@@ -16758,7 +16660,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W11" s="5" t="s">
         <v>37</v>
@@ -16767,46 +16669,46 @@
         <v>153</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="AB11" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE11" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF11" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH11" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL11" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM11" s="3" t="s">
         <v>148</v>
@@ -16967,7 +16869,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W12" s="5" t="s">
         <v>37</v>
@@ -16976,46 +16878,46 @@
         <v>153</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="AB12" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="AD12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>191</v>
       </c>
       <c r="AF12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AG12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AL12" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM12" s="3" t="s">
         <v>148</v>
@@ -17057,7 +16959,7 @@
         <v>34</v>
       </c>
       <c r="AZ12" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="BA12" s="3" t="s">
         <v>183</v>
@@ -17174,7 +17076,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="4" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
       <c r="W13" s="5" t="s">
         <v>37</v>
@@ -17182,20 +17084,48 @@
       <c r="X13" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
-      <c r="AJ13" s="3"/>
-      <c r="AK13" s="3"/>
-      <c r="AL13" s="3"/>
+      <c r="Y13" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AG13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AI13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AK13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL13" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="AM13" s="3" t="s">
         <v>148</v>
       </c>
@@ -17229,21 +17159,45 @@
       <c r="AW13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AX13" s="3"/>
+      <c r="AX13" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="AY13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AZ13" s="3"/>
-      <c r="BA13" s="3"/>
-      <c r="BB13" s="3"/>
-      <c r="BC13" s="3"/>
-      <c r="BD13" s="3"/>
-      <c r="BE13" s="3"/>
-      <c r="BF13" s="3"/>
-      <c r="BG13" s="3"/>
-      <c r="BH13" s="3"/>
-      <c r="BI13" s="3"/>
-      <c r="BJ13" s="3"/>
+      <c r="AZ13" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BA13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BB13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BE13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BF13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BG13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BH13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BI13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BJ13" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="BK13" s="3" t="s">
         <v>29</v>
       </c>
@@ -17409,7 +17363,7 @@
   <dimension ref="A1:BI13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17640,13 +17594,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -17655,19 +17609,19 @@
         <v>3</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>310</v>
+        <v>271</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>190</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>311</v>
+        <v>272</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>201</v>
@@ -17823,13 +17777,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -17837,20 +17791,16 @@
       <c r="L3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>281</v>
-      </c>
+      <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>282</v>
-      </c>
+      <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>201</v>
@@ -18006,13 +17956,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>308</v>
+        <v>236</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>309</v>
+        <v>237</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -18020,20 +17970,16 @@
       <c r="L4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>283</v>
-      </c>
+      <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>284</v>
-      </c>
+      <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>201</v>
@@ -18189,13 +18135,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -18203,20 +18149,16 @@
       <c r="L5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>285</v>
-      </c>
+      <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>286</v>
-      </c>
+      <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>201</v>
@@ -18372,13 +18314,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -18386,20 +18328,16 @@
       <c r="L6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>288</v>
-      </c>
+      <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>201</v>
@@ -18555,13 +18493,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -18569,20 +18507,16 @@
       <c r="L7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>289</v>
-      </c>
+      <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>290</v>
-      </c>
+      <c r="O7" s="3"/>
       <c r="P7" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>201</v>
@@ -18738,13 +18672,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -18752,47 +18686,43 @@
       <c r="L8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>291</v>
-      </c>
+      <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>292</v>
-      </c>
+      <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="W8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>202</v>
+        <v>264</v>
       </c>
       <c r="Y8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>203</v>
+        <v>265</v>
       </c>
       <c r="AA8" s="3" t="s">
         <v>194</v>
@@ -18921,13 +18851,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -18935,20 +18865,16 @@
       <c r="L9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>293</v>
-      </c>
+      <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>294</v>
-      </c>
+      <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>201</v>
@@ -19104,13 +19030,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -19118,20 +19044,16 @@
       <c r="L10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>295</v>
-      </c>
+      <c r="M10" s="3"/>
       <c r="N10" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>296</v>
-      </c>
+      <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>201</v>
@@ -19287,13 +19209,13 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -19301,20 +19223,16 @@
       <c r="L11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>297</v>
-      </c>
+      <c r="M11" s="3"/>
       <c r="N11" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>298</v>
-      </c>
+      <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R11" s="3" t="s">
         <v>201</v>
@@ -19470,13 +19388,13 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -19484,20 +19402,16 @@
       <c r="L12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>299</v>
-      </c>
+      <c r="M12" s="3"/>
       <c r="N12" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>300</v>
-      </c>
+      <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>201</v>
@@ -19653,13 +19567,13 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>
@@ -19667,20 +19581,16 @@
       <c r="L13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>301</v>
-      </c>
+      <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>302</v>
-      </c>
+      <c r="O13" s="3"/>
       <c r="P13" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
The category, body type change is added successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr hidePivotFieldList="1"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685DB1FF-F5D4-489A-A0FC-564B5D0F2E10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4CEB65-7C7F-41ED-97D0-2291A6474BC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="297">
   <si>
     <t>Sno</t>
   </si>
@@ -754,9 +754,6 @@
     <t>MYR 364.97</t>
   </si>
   <si>
-    <t>1000035101</t>
-  </si>
-  <si>
     <t>Policy #00000402000049390</t>
   </si>
   <si>
@@ -850,27 +847,6 @@
     <t>940309135537</t>
   </si>
   <si>
-    <t>1000035321</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049593</t>
-  </si>
-  <si>
-    <t>MYR 369.66</t>
-  </si>
-  <si>
-    <t>03-06-2025</t>
-  </si>
-  <si>
-    <t>02-06-2026</t>
-  </si>
-  <si>
-    <t>1000035464</t>
-  </si>
-  <si>
-    <t>Policy #00000402000049666</t>
-  </si>
-  <si>
     <t>MYR 8300.00</t>
   </si>
   <si>
@@ -886,26 +862,82 @@
     <t>MYR 698.15</t>
   </si>
   <si>
-    <t>020215011574</t>
-  </si>
-  <si>
-    <t>630319115042</t>
-  </si>
-  <si>
-    <t>04-06-2025</t>
-  </si>
-  <si>
-    <t>03-06-2026</t>
-  </si>
-  <si>
-    <t>960418016893</t>
+    <t>970916016684</t>
+  </si>
+  <si>
+    <t>1000037469</t>
+  </si>
+  <si>
+    <t>Policy #00000402000050854</t>
+  </si>
+  <si>
+    <t>1000037532</t>
+  </si>
+  <si>
+    <t>Policy #00000402000050884</t>
+  </si>
+  <si>
+    <t>MYR 432.03</t>
+  </si>
+  <si>
+    <t>710816015683</t>
+  </si>
+  <si>
+    <t>25-06-2025</t>
+  </si>
+  <si>
+    <t>24-06-2026</t>
+  </si>
+  <si>
+    <t>Coverage Type
+Comprehensive
+Quote Status
+Issued</t>
+  </si>
+  <si>
+    <t>JMA1147</t>
+  </si>
+  <si>
+    <t>841102016908</t>
+  </si>
+  <si>
+    <t>27-06-2025</t>
+  </si>
+  <si>
+    <t>26-06-2026</t>
+  </si>
+  <si>
+    <t>03-07-2025</t>
+  </si>
+  <si>
+    <t>02-07-2026</t>
+  </si>
+  <si>
+    <t>Coverage Type
+Comprehensive
+Quote Status
+Data Sent to JPJ</t>
+  </si>
+  <si>
+    <t>870606065570</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Body Type</t>
+  </si>
+  <si>
+    <t>SEDAN</t>
+  </si>
+  <si>
+    <t>Light Commercial Vehicle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -950,7 +982,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -993,8 +1025,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1017,11 +1055,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1081,6 +1156,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10630,6 +10717,138 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AED3F0BB-4395-4CA7-89EB-11170616EB3B}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="AD8:AE10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="57">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item m="1" x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="49"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="29">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="28">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="27">
+      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="49" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F42B4656-5BD3-4AA6-9202-8933937E4AB3}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AD3:AE7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="57">
@@ -10723,26 +10942,26 @@
     <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="29">
+    <format dxfId="35">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="34">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="33">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -10800,138 +11019,6 @@
           </reference>
           <reference field="5" count="1" selected="0">
             <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AED3F0BB-4395-4CA7-89EB-11170616EB3B}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="AD8:AE10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="57">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="49"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="35">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="34">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="33">
-      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="49" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="30">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -11835,12 +11922,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="3" max="29" style="21" width="9.140625"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="21" width="15.140625"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="32" max="16384" style="21" width="9.140625"/>
+    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="29" width="9.140625" style="21"/>
+    <col min="30" max="30" width="15.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -11965,52 +12052,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BJ13"/>
+  <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BN3" sqref="BN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="62.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.5703125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="20" width="13.140625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.42578125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.85546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5703125"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.85546875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="9.85546875"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="20.140625"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.28515625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="7.85546875"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="4.42578125"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.140625"/>
-    <col min="27" max="36" customWidth="true" width="24.140625"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="19.5703125"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" width="26.0"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="29.140625"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="28.28515625"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
-    <col min="60" max="60" customWidth="true" width="10.85546875"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="36" width="24.140625" customWidth="1"/>
+    <col min="37" max="37" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="26" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.85546875" customWidth="1"/>
+    <col min="61" max="61" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="9" customFormat="1" ht="31.5">
+    <row r="1" spans="1:64" s="9" customFormat="1" ht="31.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -12197,8 +12285,14 @@
       <c r="BJ1" s="7" t="s">
         <v>204</v>
       </c>
+      <c r="BK1" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL1" s="27" t="s">
+        <v>294</v>
+      </c>
     </row>
-    <row r="2" spans="1:62" ht="72">
+    <row r="2" spans="1:64" ht="72">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -12209,7 +12303,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -12221,13 +12315,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I2" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>286</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>287</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -12245,37 +12339,37 @@
         <v>277</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>114</v>
@@ -12383,8 +12477,14 @@
       <c r="BJ2" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK2" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL2" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="3" spans="1:62" ht="72">
+    <row r="3" spans="1:64" ht="72">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -12395,7 +12495,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -12407,13 +12507,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -12563,8 +12663,14 @@
       <c r="BJ3" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK3" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL3" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="4" spans="1:62" ht="72">
+    <row r="4" spans="1:64" ht="72">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -12575,7 +12681,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -12593,7 +12699,7 @@
         <v>223</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -12743,8 +12849,14 @@
       <c r="BJ4" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK4" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL4" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="5" spans="1:62" ht="72">
+    <row r="5" spans="1:64" ht="72">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -12755,7 +12867,7 @@
         <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -12773,7 +12885,7 @@
         <v>223</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -12923,8 +13035,14 @@
       <c r="BJ5" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK5" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL5" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="6" spans="1:62" ht="72">
+    <row r="6" spans="1:64" ht="72">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -12935,7 +13053,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>89</v>
@@ -12953,7 +13071,7 @@
         <v>223</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -13103,8 +13221,14 @@
       <c r="BJ6" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK6" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL6" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="7" spans="1:62" ht="72">
+    <row r="7" spans="1:64" ht="72">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -13115,7 +13239,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>92</v>
@@ -13133,7 +13257,7 @@
         <v>223</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -13283,8 +13407,14 @@
       <c r="BJ7" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK7" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL7" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="8" spans="1:62" ht="72">
+    <row r="8" spans="1:64" ht="72">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -13295,7 +13425,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
@@ -13313,7 +13443,7 @@
         <v>223</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -13463,8 +13593,14 @@
       <c r="BJ8" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK8" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL8" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="9" spans="1:62" ht="72">
+    <row r="9" spans="1:64" ht="72">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -13475,7 +13611,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>92</v>
@@ -13493,7 +13629,7 @@
         <v>223</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -13643,8 +13779,14 @@
       <c r="BJ9" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK9" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL9" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="10" spans="1:62" ht="72">
+    <row r="10" spans="1:64" ht="72">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -13655,7 +13797,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -13673,7 +13815,7 @@
         <v>223</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -13823,8 +13965,14 @@
       <c r="BJ10" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK10" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL10" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="11" spans="1:62" ht="72">
+    <row r="11" spans="1:64" ht="72">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -13835,7 +13983,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>56</v>
@@ -13853,7 +14001,7 @@
         <v>223</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -14003,8 +14151,14 @@
       <c r="BJ11" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK11" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL11" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="12" spans="1:62" ht="72">
+    <row r="12" spans="1:64" ht="72">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -14015,7 +14169,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>89</v>
@@ -14033,7 +14187,7 @@
         <v>223</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -14183,8 +14337,14 @@
       <c r="BJ12" s="24" t="s">
         <v>205</v>
       </c>
+      <c r="BK12" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL12" s="29" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="13" spans="1:62" ht="72">
+    <row r="13" spans="1:64" ht="72">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -14195,7 +14355,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>92</v>
@@ -14213,7 +14373,7 @@
         <v>223</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>
@@ -14362,6 +14522,12 @@
       </c>
       <c r="BJ13" s="24" t="s">
         <v>205</v>
+      </c>
+      <c r="BK13" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL13" s="29" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -14380,9 +14546,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="3" max="16384" style="21" width="9.140625"/>
+    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -14498,22 +14664,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B36D733-3F47-41DC-87DE-59145E844AA9}">
-  <dimension ref="A1:BS13"/>
+  <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView topLeftCell="P5" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="BW4" sqref="BW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="31.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.85546875"/>
-    <col min="3" max="3" customWidth="true" width="35.85546875"/>
-    <col min="11" max="11" customWidth="true" width="18.5703125"/>
-    <col min="13" max="13" style="20" width="24.7109375"/>
-    <col min="51" max="51" customWidth="true" width="27.0"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="20"/>
+    <col min="51" max="51" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="31.5" customHeight="1">
+    <row r="1" spans="1:73" ht="31.5" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -14727,8 +14893,14 @@
       <c r="BS1" s="7" t="s">
         <v>179</v>
       </c>
+      <c r="BT1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="BU1" s="7" t="s">
+        <v>294</v>
+      </c>
     </row>
-    <row r="2" spans="1:71" ht="31.5" customHeight="1">
+    <row r="2" spans="1:73" ht="31.5" customHeight="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -14798,13 +14970,13 @@
         <v>153</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>239</v>
+        <v>291</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>148</v>
@@ -14936,8 +15108,14 @@
       <c r="BS2" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT2" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU2" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="3" spans="1:71" ht="31.5" customHeight="1">
+    <row r="3" spans="1:73" ht="31.5" customHeight="1">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -15005,19 +15183,19 @@
         <v>153</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AB3" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AD3" s="3" t="s">
         <v>207</v>
@@ -15143,8 +15321,14 @@
       <c r="BS3" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT3" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU3" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="4" spans="1:71" ht="31.5" customHeight="1">
+    <row r="4" spans="1:73" ht="31.5" customHeight="1">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -15214,19 +15398,19 @@
         <v>153</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AD4" s="3" t="s">
         <v>207</v>
@@ -15352,8 +15536,14 @@
       <c r="BS4" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT4" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU4" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="5" spans="1:71" ht="31.5" customHeight="1">
+    <row r="5" spans="1:73" ht="31.5" customHeight="1">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -15421,19 +15611,19 @@
         <v>153</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AB5" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AD5" s="3" t="s">
         <v>207</v>
@@ -15559,8 +15749,14 @@
       <c r="BS5" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT5" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU5" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="6" spans="1:71" ht="31.5" customHeight="1">
+    <row r="6" spans="1:73" ht="31.5" customHeight="1">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -15630,13 +15826,13 @@
         <v>153</v>
       </c>
       <c r="Y6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="AA6" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="AB6" s="3" t="s">
         <v>148</v>
@@ -15768,8 +15964,14 @@
       <c r="BS6" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT6" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU6" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="7" spans="1:71" ht="31.5" customHeight="1">
+    <row r="7" spans="1:73" ht="31.5" customHeight="1">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -15837,19 +16039,19 @@
         <v>153</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AB7" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AD7" s="3" t="s">
         <v>207</v>
@@ -15975,8 +16177,14 @@
       <c r="BS7" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT7" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU7" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="8" spans="1:71" ht="31.5" customHeight="1">
+    <row r="8" spans="1:73" ht="31.5" customHeight="1">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -16046,19 +16254,19 @@
         <v>153</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AB8" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AD8" s="3" t="s">
         <v>207</v>
@@ -16184,8 +16392,14 @@
       <c r="BS8" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT8" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU8" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="9" spans="1:71" ht="31.5" customHeight="1">
+    <row r="9" spans="1:73" ht="31.5" customHeight="1">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -16253,19 +16467,19 @@
         <v>153</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Z9" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AB9" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AD9" s="3" t="s">
         <v>207</v>
@@ -16391,8 +16605,14 @@
       <c r="BS9" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT9" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU9" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="10" spans="1:71" ht="31.5" customHeight="1">
+    <row r="10" spans="1:73" ht="31.5" customHeight="1">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -16462,13 +16682,13 @@
         <v>153</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Z10" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AB10" s="3" t="s">
         <v>148</v>
@@ -16600,8 +16820,14 @@
       <c r="BS10" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT10" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU10" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="11" spans="1:71" ht="31.5" customHeight="1">
+    <row r="11" spans="1:73" ht="31.5" customHeight="1">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -16807,8 +17033,14 @@
       <c r="BS11" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT11" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU11" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="12" spans="1:71" ht="31.5" customHeight="1">
+    <row r="12" spans="1:73" ht="31.5" customHeight="1">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -16878,19 +17110,19 @@
         <v>153</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AB12" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AD12" s="3" t="s">
         <v>207</v>
@@ -17016,8 +17248,14 @@
       <c r="BS12" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="BT12" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU12" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="13" spans="1:71" ht="31.5" customHeight="1">
+    <row r="13" spans="1:73" ht="31.5" customHeight="1">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -17085,19 +17323,19 @@
         <v>153</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z13" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB13" s="3" t="s">
         <v>148</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AD13" s="3" t="s">
         <v>207</v>
@@ -17222,6 +17460,12 @@
       </c>
       <c r="BS13" s="19" t="s">
         <v>182</v>
+      </c>
+      <c r="BT13" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU13" s="24" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -17239,12 +17483,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="3" max="30" style="21" width="9.140625"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="33" max="16384" style="21" width="9.140625"/>
+    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="30" width="9.140625" style="21"/>
+    <col min="31" max="31" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -17360,33 +17604,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D5A56-986F-42E7-8D16-7CE6B8C79095}">
-  <dimension ref="A1:BI13"/>
+  <dimension ref="A1:BK13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="AT10" workbookViewId="0">
+      <selection activeCell="BH16" sqref="BH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7109375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="3" max="3" customWidth="true" width="22.0"/>
-    <col min="4" max="4" customWidth="true" width="13.0"/>
-    <col min="5" max="5" customWidth="true" width="14.0"/>
-    <col min="6" max="6" customWidth="true" width="15.7109375"/>
-    <col min="7" max="7" customWidth="true" width="14.7109375"/>
-    <col min="8" max="8" customWidth="true" width="15.0"/>
-    <col min="9" max="9" customWidth="true" width="14.42578125"/>
-    <col min="10" max="10" customWidth="true" width="14.0"/>
-    <col min="11" max="11" customWidth="true" width="13.5703125"/>
-    <col min="12" max="12" customWidth="true" width="13.0"/>
-    <col min="13" max="13" customWidth="true" width="17.5703125"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
-    <col min="60" max="61" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" customWidth="1"/>
+    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="31.5">
+    <row r="1" spans="1:63" ht="31.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -17570,8 +17816,14 @@
       <c r="BI1" s="7" t="s">
         <v>187</v>
       </c>
+      <c r="BJ1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>294</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" ht="72">
+    <row r="2" spans="1:63" ht="72">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -17594,13 +17846,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -17609,19 +17861,19 @@
         <v>3</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>190</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>201</v>
@@ -17753,8 +18005,14 @@
       <c r="BI2" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ2" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK2" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="3" spans="1:61" ht="72">
+    <row r="3" spans="1:63" ht="72">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -17777,13 +18035,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -17791,7 +18049,9 @@
       <c r="L3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>284</v>
+      </c>
       <c r="N3" s="3" t="s">
         <v>190</v>
       </c>
@@ -17932,8 +18192,14 @@
       <c r="BI3" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ3" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK3" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="4" spans="1:61" ht="72">
+    <row r="4" spans="1:63" ht="72">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -17962,7 +18228,7 @@
         <v>237</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -18111,8 +18377,14 @@
       <c r="BI4" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ4" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK4" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="5" spans="1:61" ht="72">
+    <row r="5" spans="1:63" ht="72">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -18141,7 +18413,7 @@
         <v>237</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>234</v>
+        <v>275</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>37</v>
@@ -18290,8 +18562,14 @@
       <c r="BI5" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ5" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK5" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="6" spans="1:61" ht="72">
+    <row r="6" spans="1:63" ht="72">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -18320,7 +18598,7 @@
         <v>237</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>37</v>
@@ -18469,8 +18747,14 @@
       <c r="BI6" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ6" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK6" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="7" spans="1:61" ht="72">
+    <row r="7" spans="1:63" ht="72">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -18499,7 +18783,7 @@
         <v>237</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>37</v>
@@ -18648,8 +18932,14 @@
       <c r="BI7" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ7" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK7" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="8" spans="1:61" ht="72">
+    <row r="8" spans="1:63" ht="72">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -18678,7 +18968,7 @@
         <v>237</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>37</v>
@@ -18692,37 +18982,37 @@
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>191</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="W8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Y8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AA8" s="3" t="s">
         <v>194</v>
@@ -18827,8 +19117,14 @@
       <c r="BI8" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ8" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK8" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="9" spans="1:61" ht="72">
+    <row r="9" spans="1:63" ht="72">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -18857,7 +19153,7 @@
         <v>237</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>37</v>
@@ -19006,8 +19302,14 @@
       <c r="BI9" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ9" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK9" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="10" spans="1:61" ht="72">
+    <row r="10" spans="1:63" ht="72">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -19036,7 +19338,7 @@
         <v>237</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>37</v>
@@ -19185,8 +19487,14 @@
       <c r="BI10" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ10" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK10" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="11" spans="1:61" ht="72">
+    <row r="11" spans="1:63" ht="72">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -19215,7 +19523,7 @@
         <v>223</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>37</v>
@@ -19364,8 +19672,14 @@
       <c r="BI11" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ11" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK11" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="12" spans="1:61" ht="72">
+    <row r="12" spans="1:63" ht="72">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -19394,7 +19708,7 @@
         <v>223</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>37</v>
@@ -19543,8 +19857,14 @@
       <c r="BI12" s="24" t="s">
         <v>189</v>
       </c>
+      <c r="BJ12" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK12" s="24" t="s">
+        <v>295</v>
+      </c>
     </row>
-    <row r="13" spans="1:61" ht="72">
+    <row r="13" spans="1:63" ht="72">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -19573,7 +19893,7 @@
         <v>223</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>37</v>
@@ -19721,6 +20041,12 @@
       </c>
       <c r="BI13" s="24" t="s">
         <v>189</v>
+      </c>
+      <c r="BJ13" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK13" s="24" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The new changes of Category, Body Type fields in New Registration Vehicle is added successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr hidePivotFieldList="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
@@ -27,7 +27,7 @@
     <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="297">
   <si>
     <t>Sno</t>
   </si>
@@ -938,6 +938,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -11922,12 +11923,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="29" width="9.140625" style="21"/>
-    <col min="30" max="30" width="15.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="3" max="29" style="21" width="9.140625"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="21" width="15.140625"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="32" max="16384" style="21" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -12060,42 +12061,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" customWidth="1"/>
-    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="36" width="24.140625" customWidth="1"/>
-    <col min="37" max="37" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="26" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.85546875" customWidth="1"/>
-    <col min="61" max="61" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="62.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.5703125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="20" width="13.140625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.42578125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="15" max="15" customWidth="true" width="24.5703125"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.85546875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="9.85546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.140625"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.28515625"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.85546875"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="4.42578125"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="24.140625"/>
+    <col min="27" max="36" customWidth="true" width="24.140625"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="19.5703125"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" width="26.0"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="29.140625"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="28.28515625"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
+    <col min="60" max="60" customWidth="true" width="10.85546875"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="9" customFormat="1" ht="31.5">
@@ -14546,9 +14547,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="3" max="16384" style="21" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -14672,11 +14673,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="31.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" style="20"/>
-    <col min="51" max="51" width="27" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="9.85546875"/>
+    <col min="3" max="3" customWidth="true" width="35.85546875"/>
+    <col min="11" max="11" customWidth="true" width="18.5703125"/>
+    <col min="13" max="13" style="20" width="24.7109375"/>
+    <col min="51" max="51" customWidth="true" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="31.5" customHeight="1">
@@ -17483,12 +17484,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="30" width="9.140625" style="21"/>
-    <col min="31" max="31" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="3" max="30" style="21" width="9.140625"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="13.140625"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
+    <col min="33" max="16384" style="21" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -17612,24 +17613,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" customWidth="1"/>
-    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="3" max="3" customWidth="true" width="22.0"/>
+    <col min="4" max="4" customWidth="true" width="13.0"/>
+    <col min="5" max="5" customWidth="true" width="14.0"/>
+    <col min="6" max="6" customWidth="true" width="15.7109375"/>
+    <col min="7" max="7" customWidth="true" width="14.7109375"/>
+    <col min="8" max="8" customWidth="true" width="15.0"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125"/>
+    <col min="10" max="10" customWidth="true" width="17.7109375"/>
+    <col min="11" max="11" customWidth="true" width="13.5703125"/>
+    <col min="12" max="12" customWidth="true" width="13.0"/>
+    <col min="13" max="13" customWidth="true" width="17.5703125"/>
+    <col min="15" max="15" customWidth="true" width="26.42578125"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
+    <col min="60" max="61" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="63" max="63" customWidth="true" width="13.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="31.5">

</xml_diff>

<commit_message>
The change in the Locator of Save & Next button is added successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4CEB65-7C7F-41ED-97D0-2291A6474BC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CEFA56-2E2F-487C-90F7-6A202065621D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DashboardRV" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="302">
   <si>
     <t>Sno</t>
   </si>
@@ -869,9 +869,6 @@
   </si>
   <si>
     <t>Policy #00000402000050854</t>
-  </si>
-  <si>
-    <t>1000037532</t>
   </si>
   <si>
     <t>Policy #00000402000050884</t>
@@ -907,12 +904,6 @@
     <t>26-06-2026</t>
   </si>
   <si>
-    <t>03-07-2025</t>
-  </si>
-  <si>
-    <t>02-07-2026</t>
-  </si>
-  <si>
     <t>Coverage Type
 Comprehensive
 Quote Status
@@ -932,6 +923,30 @@
   </si>
   <si>
     <t>Light Commercial Vehicle</t>
+  </si>
+  <si>
+    <t>PMJ3951</t>
+  </si>
+  <si>
+    <t>930701015792</t>
+  </si>
+  <si>
+    <t>AJG6911</t>
+  </si>
+  <si>
+    <t>790618-08-6264</t>
+  </si>
+  <si>
+    <t>08-07-2025</t>
+  </si>
+  <si>
+    <t>07-07-2026</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>730617105764</t>
   </si>
 </sst>
 </file>
@@ -939,7 +954,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,6 +995,12 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1097,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1155,9 +1176,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1169,6 +1187,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11932,50 +11954,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:31">
       <c r="AD3" s="21" t="s">
@@ -12055,8 +12077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BN3" sqref="BN3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12070,7 +12092,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="15.5703125"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="20" width="13.140625"/>
+    <col min="10" max="10" customWidth="true" style="20" width="16.0"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="19.42578125"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="15.85546875"/>
@@ -12286,11 +12308,11 @@
       <c r="BJ1" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="BK1" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="BL1" s="27" t="s">
-        <v>294</v>
+      <c r="BK1" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL1" s="26" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="72">
@@ -12303,8 +12325,8 @@
       <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>285</v>
+      <c r="D2" s="29" t="s">
+        <v>296</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -12316,13 +12338,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>286</v>
+        <v>299</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>297</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -12478,11 +12500,11 @@
       <c r="BJ2" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK2" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL2" s="29" t="s">
-        <v>295</v>
+      <c r="BK2" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL2" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="72">
@@ -12496,7 +12518,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -12508,13 +12530,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="J3" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -12664,11 +12686,11 @@
       <c r="BJ3" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK3" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL3" s="29" t="s">
-        <v>295</v>
+      <c r="BK3" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL3" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:64" ht="72">
@@ -12682,7 +12704,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>268</v>
+        <v>294</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -12700,7 +12722,7 @@
         <v>223</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>269</v>
+        <v>295</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -12850,11 +12872,11 @@
       <c r="BJ4" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK4" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL4" s="29" t="s">
-        <v>295</v>
+      <c r="BK4" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL4" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:64" ht="72">
@@ -13036,11 +13058,11 @@
       <c r="BJ5" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK5" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL5" s="29" t="s">
-        <v>295</v>
+      <c r="BK5" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL5" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="72">
@@ -13222,11 +13244,11 @@
       <c r="BJ6" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK6" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL6" s="29" t="s">
-        <v>295</v>
+      <c r="BK6" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL6" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:64" ht="72">
@@ -13408,11 +13430,11 @@
       <c r="BJ7" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK7" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL7" s="29" t="s">
-        <v>295</v>
+      <c r="BK7" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL7" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:64" ht="72">
@@ -13594,11 +13616,11 @@
       <c r="BJ8" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK8" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL8" s="29" t="s">
-        <v>295</v>
+      <c r="BK8" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL8" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:64" ht="72">
@@ -13780,11 +13802,11 @@
       <c r="BJ9" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK9" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL9" s="29" t="s">
-        <v>295</v>
+      <c r="BK9" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL9" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:64" ht="72">
@@ -13966,11 +13988,11 @@
       <c r="BJ10" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK10" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL10" s="29" t="s">
-        <v>295</v>
+      <c r="BK10" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL10" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:64" ht="72">
@@ -14152,11 +14174,11 @@
       <c r="BJ11" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK11" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL11" s="29" t="s">
-        <v>295</v>
+      <c r="BK11" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL11" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:64" ht="72">
@@ -14338,11 +14360,11 @@
       <c r="BJ12" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK12" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL12" s="29" t="s">
-        <v>295</v>
+      <c r="BK12" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL12" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:64" ht="72">
@@ -14524,11 +14546,11 @@
       <c r="BJ13" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="BK13" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="BL13" s="29" t="s">
-        <v>295</v>
+      <c r="BK13" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="BL13" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -14553,50 +14575,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:33">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="9" spans="1:33">
       <c r="AF9" s="21" t="s">
@@ -14895,10 +14917,10 @@
         <v>179</v>
       </c>
       <c r="BT1" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BU1" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:73" ht="31.5" customHeight="1">
@@ -14971,7 +14993,7 @@
         <v>153</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>210</v>
@@ -15110,10 +15132,10 @@
         <v>182</v>
       </c>
       <c r="BT2" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU2" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:73" ht="31.5" customHeight="1">
@@ -15323,10 +15345,10 @@
         <v>182</v>
       </c>
       <c r="BT3" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU3" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:73" ht="31.5" customHeight="1">
@@ -15538,10 +15560,10 @@
         <v>182</v>
       </c>
       <c r="BT4" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU4" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:73" ht="31.5" customHeight="1">
@@ -15751,10 +15773,10 @@
         <v>182</v>
       </c>
       <c r="BT5" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU5" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:73" ht="31.5" customHeight="1">
@@ -15966,10 +15988,10 @@
         <v>182</v>
       </c>
       <c r="BT6" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU6" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:73" ht="31.5" customHeight="1">
@@ -16179,10 +16201,10 @@
         <v>182</v>
       </c>
       <c r="BT7" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU7" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:73" ht="31.5" customHeight="1">
@@ -16394,10 +16416,10 @@
         <v>182</v>
       </c>
       <c r="BT8" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU8" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:73" ht="31.5" customHeight="1">
@@ -16607,10 +16629,10 @@
         <v>182</v>
       </c>
       <c r="BT9" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU9" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:73" ht="31.5" customHeight="1">
@@ -16822,10 +16844,10 @@
         <v>182</v>
       </c>
       <c r="BT10" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU10" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:73" ht="31.5" customHeight="1">
@@ -17035,10 +17057,10 @@
         <v>182</v>
       </c>
       <c r="BT11" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU11" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:73" ht="31.5" customHeight="1">
@@ -17250,10 +17272,10 @@
         <v>182</v>
       </c>
       <c r="BT12" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU12" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:73" ht="31.5" customHeight="1">
@@ -17463,10 +17485,10 @@
         <v>182</v>
       </c>
       <c r="BT13" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BU13" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -17493,50 +17515,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:32">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="9" spans="1:32">
       <c r="AE9" s="21" t="s">
@@ -17607,8 +17629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D5A56-986F-42E7-8D16-7CE6B8C79095}">
   <dimension ref="A1:BK13"/>
   <sheetViews>
-    <sheetView topLeftCell="AT10" workbookViewId="0">
-      <selection activeCell="BH16" sqref="BH16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17627,6 +17649,11 @@
     <col min="12" max="12" customWidth="true" width="13.0"/>
     <col min="13" max="13" customWidth="true" width="17.5703125"/>
     <col min="15" max="15" customWidth="true" width="26.42578125"/>
+    <col min="16" max="16" customWidth="true" width="13.85546875"/>
+    <col min="17" max="17" customWidth="true" width="14.140625"/>
+    <col min="18" max="18" customWidth="true" width="15.0"/>
+    <col min="25" max="25" customWidth="true" width="12.42578125"/>
+    <col min="26" max="26" customWidth="true" width="22.85546875"/>
     <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
     <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
     <col min="60" max="61" bestFit="true" customWidth="true" width="16.140625"/>
@@ -17818,10 +17845,10 @@
         <v>187</v>
       </c>
       <c r="BJ1" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BK1" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:63" ht="72">
@@ -17847,13 +17874,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -17862,19 +17889,19 @@
         <v>3</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>190</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>201</v>
@@ -18007,10 +18034,10 @@
         <v>189</v>
       </c>
       <c r="BJ2" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK2" s="24" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:63" ht="72">
@@ -18036,13 +18063,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>37</v>
@@ -18051,7 +18078,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>190</v>
@@ -18194,10 +18221,10 @@
         <v>189</v>
       </c>
       <c r="BJ3" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK3" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:63" ht="72">
@@ -18229,7 +18256,7 @@
         <v>237</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -18379,10 +18406,10 @@
         <v>189</v>
       </c>
       <c r="BJ4" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK4" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:63" ht="72">
@@ -18564,10 +18591,10 @@
         <v>189</v>
       </c>
       <c r="BJ5" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK5" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="72">
@@ -18749,10 +18776,10 @@
         <v>189</v>
       </c>
       <c r="BJ6" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK6" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:63" ht="72">
@@ -18934,10 +18961,10 @@
         <v>189</v>
       </c>
       <c r="BJ7" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK7" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="72">
@@ -19119,10 +19146,10 @@
         <v>189</v>
       </c>
       <c r="BJ8" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK8" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:63" ht="72">
@@ -19304,10 +19331,10 @@
         <v>189</v>
       </c>
       <c r="BJ9" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK9" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:63" ht="72">
@@ -19489,10 +19516,10 @@
         <v>189</v>
       </c>
       <c r="BJ10" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK10" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:63" ht="72">
@@ -19674,10 +19701,10 @@
         <v>189</v>
       </c>
       <c r="BJ11" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK11" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:63" ht="72">
@@ -19859,10 +19886,10 @@
         <v>189</v>
       </c>
       <c r="BJ12" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK12" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:63" ht="72">
@@ -20044,10 +20071,10 @@
         <v>189</v>
       </c>
       <c r="BJ13" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BK13" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The update in pom.xml, testng.xml is done successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr hidePivotFieldList="1"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CEFA56-2E2F-487C-90F7-6A202065621D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005005E7-17E6-48DE-9054-AFF997B9C1D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="304">
   <si>
     <t>Sno</t>
   </si>
@@ -931,12 +931,6 @@
     <t>930701015792</t>
   </si>
   <si>
-    <t>AJG6911</t>
-  </si>
-  <si>
-    <t>790618-08-6264</t>
-  </si>
-  <si>
     <t>08-07-2025</t>
   </si>
   <si>
@@ -947,14 +941,25 @@
   </si>
   <si>
     <t>730617105764</t>
+  </si>
+  <si>
+    <t>09-07-2025</t>
+  </si>
+  <si>
+    <t>08-07-2026</t>
+  </si>
+  <si>
+    <t>AJL9647</t>
+  </si>
+  <si>
+    <t>841025086274</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,12 +1000,6 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1185,12 +1184,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11060,6 +11061,148 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E65630C9-EB18-432C-A1B4-98C52238F2EB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="AF14:AG16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="68">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="61"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="65" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="17">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea field="61" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="61" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{591533EA-EEAC-4542-9EEA-CD8FE30E3B88}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AF9:AG12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="68">
@@ -11159,26 +11302,26 @@
     <dataField name="Sum of Value" fld="65" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="17">
+    <format dxfId="23">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="21">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="17" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -11212,148 +11355,6 @@
           </reference>
           <reference field="17" count="1" selected="0">
             <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E65630C9-EB18-432C-A1B4-98C52238F2EB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="AF14:AG16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="68">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="61"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="65" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="23">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="21">
-      <pivotArea field="61" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="61" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -11945,59 +11946,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="3" max="29" style="21" width="9.140625"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="21" width="15.140625"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="32" max="16384" style="21" width="9.140625"/>
+    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="29" width="9.140625" style="21"/>
+    <col min="30" max="30" width="15.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="3" spans="1:31">
       <c r="AD3" s="21" t="s">
@@ -12077,48 +12078,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BM3" sqref="BM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="62.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.5703125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625"/>
-    <col min="10" max="10" customWidth="true" style="20" width="16.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.42578125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.85546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="15" max="15" customWidth="true" width="24.5703125"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.85546875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="9.85546875"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="20.140625"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.28515625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.85546875"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="7.85546875"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="4.42578125"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.140625"/>
-    <col min="27" max="36" customWidth="true" width="24.140625"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="19.5703125"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" width="26.0"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="29.140625"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="28.28515625"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
-    <col min="60" max="60" customWidth="true" width="10.85546875"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="20" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="36" width="24.140625" customWidth="1"/>
+    <col min="37" max="37" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="26" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.85546875" customWidth="1"/>
+    <col min="61" max="61" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.28515625" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="9" customFormat="1" ht="31.5">
@@ -12325,8 +12326,8 @@
       <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>296</v>
+      <c r="D2" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -12338,13 +12339,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>297</v>
+        <v>301</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>303</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -12503,8 +12504,8 @@
       <c r="BK2" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL2" s="28" t="s">
-        <v>292</v>
+      <c r="BL2" s="29" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="72">
@@ -12689,7 +12690,7 @@
       <c r="BK3" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL3" s="28" t="s">
+      <c r="BL3" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -12875,7 +12876,7 @@
       <c r="BK4" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL4" s="28" t="s">
+      <c r="BL4" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13061,7 +13062,7 @@
       <c r="BK5" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL5" s="28" t="s">
+      <c r="BL5" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13247,7 +13248,7 @@
       <c r="BK6" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL6" s="28" t="s">
+      <c r="BL6" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13433,7 +13434,7 @@
       <c r="BK7" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL7" s="28" t="s">
+      <c r="BL7" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13619,7 +13620,7 @@
       <c r="BK8" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL8" s="28" t="s">
+      <c r="BL8" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13805,7 +13806,7 @@
       <c r="BK9" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL9" s="28" t="s">
+      <c r="BL9" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13991,7 +13992,7 @@
       <c r="BK10" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL10" s="28" t="s">
+      <c r="BL10" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14177,7 +14178,7 @@
       <c r="BK11" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL11" s="28" t="s">
+      <c r="BL11" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14363,7 +14364,7 @@
       <c r="BK12" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL12" s="28" t="s">
+      <c r="BL12" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14549,7 +14550,7 @@
       <c r="BK13" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL13" s="28" t="s">
+      <c r="BL13" s="29" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14569,56 +14570,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="3" max="16384" style="21" width="9.140625"/>
+    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:33">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="9" spans="1:33">
       <c r="AF9" s="21" t="s">
@@ -14690,16 +14691,16 @@
   <dimension ref="A1:BU13"/>
   <sheetViews>
     <sheetView topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="BW4" sqref="BW4"/>
+      <selection activeCell="BV3" sqref="BV3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="31.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.85546875"/>
-    <col min="3" max="3" customWidth="true" width="35.85546875"/>
-    <col min="11" max="11" customWidth="true" width="18.5703125"/>
-    <col min="13" max="13" style="20" width="24.7109375"/>
-    <col min="51" max="51" customWidth="true" width="27.0"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="20"/>
+    <col min="51" max="51" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="31.5" customHeight="1">
@@ -15135,7 +15136,7 @@
         <v>293</v>
       </c>
       <c r="BU2" s="24" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:73" ht="31.5" customHeight="1">
@@ -17506,59 +17507,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="3" max="30" style="21" width="9.140625"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="21" width="13.140625"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="21" width="12.7109375"/>
-    <col min="33" max="16384" style="21" width="9.140625"/>
+    <col min="1" max="1" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="30" width="9.140625" style="21"/>
+    <col min="31" max="31" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:32">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="9" spans="1:32">
       <c r="AE9" s="21" t="s">
@@ -17629,35 +17630,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D5A56-986F-42E7-8D16-7CE6B8C79095}">
   <dimension ref="A1:BK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7109375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="3" max="3" customWidth="true" width="22.0"/>
-    <col min="4" max="4" customWidth="true" width="13.0"/>
-    <col min="5" max="5" customWidth="true" width="14.0"/>
-    <col min="6" max="6" customWidth="true" width="15.7109375"/>
-    <col min="7" max="7" customWidth="true" width="14.7109375"/>
-    <col min="8" max="8" customWidth="true" width="15.0"/>
-    <col min="9" max="9" customWidth="true" width="14.42578125"/>
-    <col min="10" max="10" customWidth="true" width="17.7109375"/>
-    <col min="11" max="11" customWidth="true" width="13.5703125"/>
-    <col min="12" max="12" customWidth="true" width="13.0"/>
-    <col min="13" max="13" customWidth="true" width="17.5703125"/>
-    <col min="15" max="15" customWidth="true" width="26.42578125"/>
-    <col min="16" max="16" customWidth="true" width="13.85546875"/>
-    <col min="17" max="17" customWidth="true" width="14.140625"/>
-    <col min="18" max="18" customWidth="true" width="15.0"/>
-    <col min="25" max="25" customWidth="true" width="12.42578125"/>
-    <col min="26" max="26" customWidth="true" width="22.85546875"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.28515625"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.85546875"/>
-    <col min="60" max="61" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="63" max="63" customWidth="true" width="13.0"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" customWidth="1"/>
+    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="31.5">
@@ -17874,13 +17875,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I2" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>301</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -18037,7 +18038,7 @@
         <v>293</v>
       </c>
       <c r="BK2" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:63" ht="72">

</xml_diff>

<commit_message>
The changes in TO class is updated successfully, extends TOBaseinstead of RVBase earlier
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005005E7-17E6-48DE-9054-AFF997B9C1D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD290CC-4F85-449A-8AFE-3DB7D65E2967}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DashboardRV" sheetId="7" r:id="rId1"/>
@@ -931,28 +931,28 @@
     <t>930701015792</t>
   </si>
   <si>
-    <t>08-07-2025</t>
-  </si>
-  <si>
-    <t>07-07-2026</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
     <t>730617105764</t>
   </si>
   <si>
-    <t>09-07-2025</t>
-  </si>
-  <si>
-    <t>08-07-2026</t>
-  </si>
-  <si>
-    <t>AJL9647</t>
-  </si>
-  <si>
-    <t>841025086274</t>
+    <t>02-09-2025</t>
+  </si>
+  <si>
+    <t>01-09-2026</t>
+  </si>
+  <si>
+    <t>10-07-2025</t>
+  </si>
+  <si>
+    <t>09-07-2026</t>
+  </si>
+  <si>
+    <t>W664V</t>
+  </si>
+  <si>
+    <t>700311055306</t>
   </si>
 </sst>
 </file>
@@ -1184,14 +1184,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11373,6 +11373,137 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4835F9D5-316A-469B-AC80-1739299B9E0F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="AE14:AF16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="57">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="49"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="5">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="49" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{237DE21D-C108-407B-9CCD-EB11944F6790}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AE9:AF12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="57">
@@ -11462,26 +11593,26 @@
     <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="5">
+    <format dxfId="11">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="9">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -11527,137 +11658,6 @@
           </reference>
           <reference field="5" count="1" selected="0">
             <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4835F9D5-316A-469B-AC80-1739299B9E0F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="AE14:AF16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="57">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="49"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="11">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="10">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="9">
-      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="49" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -11955,50 +11955,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:31">
       <c r="AD3" s="21" t="s">
@@ -12078,8 +12078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BM3" sqref="BM3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12119,7 +12119,7 @@
     <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="10.85546875" customWidth="1"/>
     <col min="61" max="61" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.28515625" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="9" customFormat="1" ht="31.5">
@@ -12339,10 +12339,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>303</v>
@@ -12504,8 +12504,8 @@
       <c r="BK2" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL2" s="29" t="s">
-        <v>298</v>
+      <c r="BL2" s="28" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="72">
@@ -12690,7 +12690,7 @@
       <c r="BK3" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL3" s="29" t="s">
+      <c r="BL3" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -12876,7 +12876,7 @@
       <c r="BK4" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL4" s="29" t="s">
+      <c r="BL4" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13062,7 +13062,7 @@
       <c r="BK5" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL5" s="29" t="s">
+      <c r="BL5" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13248,7 +13248,7 @@
       <c r="BK6" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL6" s="29" t="s">
+      <c r="BL6" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13434,7 +13434,7 @@
       <c r="BK7" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL7" s="29" t="s">
+      <c r="BL7" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13620,7 +13620,7 @@
       <c r="BK8" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL8" s="29" t="s">
+      <c r="BL8" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13806,7 +13806,7 @@
       <c r="BK9" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL9" s="29" t="s">
+      <c r="BL9" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -13992,7 +13992,7 @@
       <c r="BK10" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL10" s="29" t="s">
+      <c r="BL10" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14178,7 +14178,7 @@
       <c r="BK11" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL11" s="29" t="s">
+      <c r="BL11" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14364,7 +14364,7 @@
       <c r="BK12" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL12" s="29" t="s">
+      <c r="BL12" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14550,7 +14550,7 @@
       <c r="BK13" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="BL13" s="29" t="s">
+      <c r="BL13" s="28" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14576,50 +14576,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:33">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="9" spans="1:33">
       <c r="AF9" s="21" t="s">
@@ -15136,7 +15136,7 @@
         <v>293</v>
       </c>
       <c r="BU2" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:73" ht="31.5" customHeight="1">
@@ -17516,50 +17516,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:32">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="9" spans="1:32">
       <c r="AE9" s="21" t="s">
@@ -17630,7 +17630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D5A56-986F-42E7-8D16-7CE6B8C79095}">
   <dimension ref="A1:BK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BI3" sqref="BI3"/>
     </sheetView>
   </sheetViews>
@@ -17875,13 +17875,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I2" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>299</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -18038,7 +18038,7 @@
         <v>293</v>
       </c>
       <c r="BK2" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:63" ht="72">

</xml_diff>

<commit_message>
The changes in the locator of IssuePolicy, Policy Letter is updated in RV, TO successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PrivateCar.xlsx
+++ b/src/test/resources/TestData/PrivateCar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\PrivateCar-UAT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD290CC-4F85-449A-8AFE-3DB7D65E2967}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6612EC9-4897-4468-A755-0B6664B716F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,22 +937,22 @@
     <t>730617105764</t>
   </si>
   <si>
-    <t>02-09-2025</t>
-  </si>
-  <si>
-    <t>01-09-2026</t>
-  </si>
-  <si>
     <t>10-07-2025</t>
   </si>
   <si>
     <t>09-07-2026</t>
   </si>
   <si>
-    <t>W664V</t>
-  </si>
-  <si>
-    <t>700311055306</t>
+    <t>11-07-2025</t>
+  </si>
+  <si>
+    <t>10-07-2026</t>
+  </si>
+  <si>
+    <t>780322135961</t>
+  </si>
+  <si>
+    <t>SS8033X</t>
   </si>
 </sst>
 </file>
@@ -11373,137 +11373,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4835F9D5-316A-469B-AC80-1739299B9E0F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="AE14:AF16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="57">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="49"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="5">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="3">
-      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="49" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{237DE21D-C108-407B-9CCD-EB11944F6790}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AE9:AF12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="57">
@@ -11593,26 +11462,26 @@
     <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="11">
+    <format dxfId="5">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="3">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -11658,6 +11527,137 @@
           </reference>
           <reference field="5" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4835F9D5-316A-469B-AC80-1739299B9E0F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="AE14:AF16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="57">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="49"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="52" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="11">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="49" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="49" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -12079,7 +12079,7 @@
   <dimension ref="A1:BL13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12327,7 +12327,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>56</v>
@@ -12339,13 +12339,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>37</v>
@@ -17875,10 +17875,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>297</v>

</xml_diff>